<commit_message>
test pandas with gravity
</commit_message>
<xml_diff>
--- a/pendulum/work_on_memory/memory_raw_data.xlsx
+++ b/pendulum/work_on_memory/memory_raw_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sky/Documents/Work Info/Research Assistant/deap_experiments/pendulum/memory_pendulum_work_on/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sky/Documents/Work Info/Research Assistant/deap_experiments/pendulum/work_on_memory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8B513F5-4747-7945-A00D-F73DC786B92B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3912739-DF93-5245-8A32-E3FE662A6DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" xr2:uid="{F0179072-8820-814B-8D68-6BA03E148DB0}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15680" xr2:uid="{F0179072-8820-814B-8D68-6BA03E148DB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
   <si>
     <t>Row 1</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>ads</t>
   </si>
 </sst>
 </file>
@@ -390,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A27434-6935-3349-A2A1-C839CB3E3958}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -403,6 +409,36 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Change mut from .5 to 0.75
</commit_message>
<xml_diff>
--- a/pendulum/work_on_memory/memory_raw_data.xlsx
+++ b/pendulum/work_on_memory/memory_raw_data.xlsx
@@ -1,42 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10514"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sky/Documents/Work Info/Research Assistant/deap_experiments/pendulum/work_on_memory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3912739-DF93-5245-8A32-E3FE662A6DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5370DAEE-1BD6-9148-B114-B5D95F75CAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15680" xr2:uid="{F0179072-8820-814B-8D68-6BA03E148DB0}"/>
+    <workbookView xWindow="480" yWindow="500" windowWidth="18200" windowHeight="8500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>Row 1</t>
   </si>
@@ -53,7 +37,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -87,7 +71,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -134,20 +118,20 @@
         <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -175,31 +159,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -227,23 +194,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -255,156 +205,184 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A27434-6935-3349-A2A1-C839CB3E3958}">
-  <dimension ref="A1:A7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,11 +409,6 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Create memory_grav excel sheet to write to
</commit_message>
<xml_diff>
--- a/pendulum/work_on_memory/memory_raw_data.xlsx
+++ b/pendulum/work_on_memory/memory_raw_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sky/Documents/Work Info/Research Assistant/deap_experiments/pendulum/work_on_memory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5370DAEE-1BD6-9148-B114-B5D95F75CAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E5FDB4-61FB-7640-8A3E-DA38EFF09C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="500" windowWidth="18200" windowHeight="8500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,15 +20,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
-  <si>
-    <t>Row 1</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>ads</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>limit(sin(a2), limit(0, read(a0, a1), sub(read(a0, a1), add(write(a0, conditional(protectedDiv(0, protectedDiv(cos(a2), sin(abs(sub(cos(0), a1))))), a2), a2), a1))), protectedLog(a2))</t>
+  </si>
+  <si>
+    <t>sub(read(a0, a1), add(add(add(a2, a2), a2), add(a2, add(add(a2, write(a0, sin(0), add(sin(read(a0, limit(a2, protectedLog(a2), a2))), a2))), add(a2, sub(protectedDiv(abs(a2), a2), read(a0, read(a0, cos(conditional(a1, 0))))))))))</t>
+  </si>
+  <si>
+    <t>protectedDiv(add(read(a0, read(a0, sub(sin(add(read(a0, a1), protectedDiv(0, a1))), protectedDiv(0, a2)))), a2), conditional(sin(sin(read(a0, a1))), write(a0, limit(protectedLog(read(a0, add(add(conditional(abs(sin(a1)), a1), a2), sin(sin(a2))))), abs(limit(0, read(a0, a2), 0)), conditional(protectedDiv(0, a1), protectedDiv(a1, conditional(a2, read(a0, 0))))), a2)))</t>
+  </si>
+  <si>
+    <t>sub(sub(limit(a2, read(a0, a2), protectedLog(read(a0, abs(0)))), a2), add(write(a0, protectedLog(sub(conditional(a1, a2), sin(a2))), write(a0, protectedDiv(a1, limit(0, 0, limit(write(a0, a1, write(a0, 0, a2)), a2, a2))), a2)), limit(sin(cos(sub(protectedLog(abs(a2)), a2))), sub(0, limit(a2, a1, 0)), a2)))</t>
+  </si>
+  <si>
+    <t>sub(sub(read(a0, a1), add(write(a0, abs(a2), protectedDiv(add(a2, a2), protectedLog(write(a0, sin(cos(0)), abs(a1))))), cos(read(a0, read(a0, abs(sub(a1, conditional(limit(a2, limit(0, a1, a2), a2), a1)))))))), sub(a2, protectedLog(a2)))</t>
+  </si>
+  <si>
+    <t>sub(read(a0, a2), write(a0, sub(conditional(write(a0, a1, protectedLog(conditional(a1, protectedLog(a1)))), add(abs(0), sub(abs(write(a0, a1, a1)), add(protectedDiv(a2, a2), limit(0, 0, 0))))), conditional(0, conditional(conditional(a2, abs(a1)), a1))), protectedDiv(a2, conditional(sub(a2, sin(sin(write(a0, abs(conditional(sin(a1), 0)), a2)))), a2))))</t>
+  </si>
+  <si>
+    <t>sub(sub(0, read(a0, a1)), add(protectedDiv(conditional(a2, read(a0, read(a0, a1))), a2), add(write(a0, a1, sin(a2)), a2)))</t>
+  </si>
+  <si>
+    <t>sub(protectedDiv(sub(protectedDiv(conditional(read(a0, a2), a2), a2), sin(limit(0, 0, a1))), cos(sub(write(a0, 0, a2), cos(limit(cos(sin(a2)), 0, read(a0, 0)))))), a2)</t>
+  </si>
+  <si>
+    <t>sub(sub(read(a0, 0), protectedDiv(limit(sin(a1), protectedDiv(a2, protectedDiv(read(a0, a2), a1)), protectedLog(read(a0, a2))), a2)), write(a0, a2, a2))</t>
+  </si>
+  <si>
+    <t>protectedDiv(sub(sub(0, write(a0, a2, conditional(conditional(a2, 0), sin(read(a0, 0))))), write(a0, protectedDiv(a1, a1), conditional(conditional(a2, 0), read(a0, 0)))), a2)</t>
   </si>
 </sst>
 </file>
@@ -371,10 +392,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -382,34 +403,84 @@
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>-846</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>-435</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>-151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>-392</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>-151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>-457</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>-165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>-830</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>-165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>-125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make change to excel
</commit_message>
<xml_diff>
--- a/pendulum/work_on_memory/memory_raw_data.xlsx
+++ b/pendulum/work_on_memory/memory_raw_data.xlsx
@@ -43,7 +43,7 @@
     <t>protectedDiv(sub(a2, read(a0, read(a0, a1))), protectedLog(conditional(protectedDiv(a1, cos(a2)), limit(protectedDiv(sin(sub(a2, a2)), protectedLog(limit(a1, protectedDiv(a1, a2), a2))), a1, protectedLog(write(a0, read(a0, cos(conditional(a2, read(a0, a1)))), write(a0, sin(a1), sin(sin(a2)))))))))</t>
   </si>
   <si>
-    <t>sub(write(a0, 0, protectedDiv(read(a0, a1), cos(limit(write(a0, cos(abs(limit(a1, abs(abs(0)), 0))), a1), sub(a2, 0), a1)))), write(a0, add(abs(cos(add(a1, a1))), sub(add(sub(sin(sub(0, a1)), 0), 0), a1)), limit(0, protectedDiv(limit(read(a0, read(a0, a2)), read(a0, sub(a2, a2)), sub(0, sub(abs(write(a0, a1, conditional(protectedDiv(a1, protectedLog(cos(a2))), a2))), a2))), a2), protectedDiv(read(a0, add(a2, a2)), protectedLog(cos(a2))))))</t>
+    <t>Should not be here</t>
   </si>
 </sst>
 </file>
@@ -61,7 +61,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -419,7 +419,7 @@
     <col min="2" max="2" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -427,7 +427,7 @@
         <v>-236</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -435,7 +435,7 @@
         <v>-977</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -443,7 +443,7 @@
         <v>-193</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -451,7 +451,7 @@
         <v>-134</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -459,7 +459,7 @@
         <v>-224</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -467,7 +467,7 @@
         <v>-938</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -475,7 +475,7 @@
         <v>-477</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -483,7 +483,7 @@
         <v>-116</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -491,7 +491,7 @@
         <v>-117</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>